<commit_message>
FTDI chip hooked up for USB UART
</commit_message>
<xml_diff>
--- a/Documentation/Interface Connector Pinout.xlsx
+++ b/Documentation/Interface Connector Pinout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\personal\mino\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\msx\amino\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +239,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,29 +695,29 @@
       <c r="J2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>4</v>
+      <c r="R2" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>4</v>
@@ -726,10 +734,10 @@
       <c r="W2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="12" t="s">
+      <c r="X2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Z2" s="12" t="s">
@@ -744,8 +752,8 @@
       <c r="AC2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="5" t="s">
-        <v>0</v>
+      <c r="AD2" s="12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -874,23 +882,23 @@
       <c r="K4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>12</v>
+      <c r="L4" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>4</v>
+      <c r="Q4" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>4</v>
@@ -910,11 +918,11 @@
       <c r="W4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>0</v>
+      <c r="X4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="Z4" s="12" t="s">
         <v>4</v>
@@ -994,41 +1002,192 @@
       <c r="H15" s="7"/>
       <c r="I15" s="8"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="7"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="23"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AC16" s="23"/>
+      <c r="AD16" s="23"/>
+    </row>
+    <row r="17" spans="8:30" x14ac:dyDescent="0.3">
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="23"/>
+    </row>
+    <row r="18" spans="8:30" x14ac:dyDescent="0.3">
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
+      <c r="AC18" s="26"/>
+      <c r="AD18" s="23"/>
+    </row>
+    <row r="19" spans="8:30" x14ac:dyDescent="0.3">
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23"/>
+    </row>
+    <row r="20" spans="8:30" x14ac:dyDescent="0.3">
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23"/>
+    </row>
+    <row r="21" spans="8:30" x14ac:dyDescent="0.3">
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+    </row>
+    <row r="22" spans="8:30" x14ac:dyDescent="0.3">
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Notes review completed, prep for netlist review
</commit_message>
<xml_diff>
--- a/Documentation/Interface Connector Pinout.xlsx
+++ b/Documentation/Interface Connector Pinout.xlsx
@@ -564,7 +564,7 @@
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,11 +740,11 @@
       <c r="Y2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>4</v>
+      <c r="Z2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="AB2" s="12" t="s">
         <v>4</v>
@@ -924,14 +924,14 @@
       <c r="Y4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="12" t="s">
-        <v>4</v>
+      <c r="Z4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="AC4" s="12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Swapping and fanning out the BGA
</commit_message>
<xml_diff>
--- a/Documentation/Interface Connector Pinout.xlsx
+++ b/Documentation/Interface Connector Pinout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="INTF" sheetId="1" r:id="rId1"/>
@@ -564,15 +564,15 @@
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="30" width="6.109375" customWidth="1"/>
+    <col min="1" max="30" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -664,7 +664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -740,8 +740,8 @@
       <c r="Y2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="6" t="s">
-        <v>4</v>
+      <c r="Z2" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="AA2" s="5" t="s">
         <v>0</v>
@@ -756,7 +756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -848,7 +848,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -927,8 +927,8 @@
       <c r="Z4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="6" t="s">
-        <v>4</v>
+      <c r="AA4" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="AB4" s="5" t="s">
         <v>0</v>
@@ -940,49 +940,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="19"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="22"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="14"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="18"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="AC15" s="23"/>
       <c r="AD15" s="23"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1048,7 +1048,7 @@
       <c r="AC16" s="23"/>
       <c r="AD16" s="23"/>
     </row>
-    <row r="17" spans="8:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:30" x14ac:dyDescent="0.25">
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1073,7 +1073,7 @@
       <c r="AC17" s="23"/>
       <c r="AD17" s="23"/>
     </row>
-    <row r="18" spans="8:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:30" x14ac:dyDescent="0.25">
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1098,7 +1098,7 @@
       <c r="AC18" s="26"/>
       <c r="AD18" s="23"/>
     </row>
-    <row r="19" spans="8:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:30" x14ac:dyDescent="0.25">
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1123,7 +1123,7 @@
       <c r="AC19" s="23"/>
       <c r="AD19" s="23"/>
     </row>
-    <row r="20" spans="8:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:30" x14ac:dyDescent="0.25">
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23"/>
@@ -1145,7 +1145,7 @@
       <c r="AC20" s="23"/>
       <c r="AD20" s="23"/>
     </row>
-    <row r="21" spans="8:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:30" x14ac:dyDescent="0.25">
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23"/>
@@ -1167,7 +1167,7 @@
       <c r="AC21" s="23"/>
       <c r="AD21" s="23"/>
     </row>
-    <row r="22" spans="8:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:30" x14ac:dyDescent="0.25">
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>

</xml_diff>

<commit_message>
Review notes, begin transition to MoM design
</commit_message>
<xml_diff>
--- a/Documentation/Interface Connector Pinout.xlsx
+++ b/Documentation/Interface Connector Pinout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
   <si>
     <t>GND</t>
   </si>
@@ -44,22 +44,13 @@
     <t>MCU</t>
   </si>
   <si>
-    <t>BLE</t>
-  </si>
-  <si>
     <t>D+</t>
   </si>
   <si>
     <t>D-</t>
   </si>
   <si>
-    <t>PDI</t>
-  </si>
-  <si>
     <t>CLK</t>
-  </si>
-  <si>
-    <t>DAT</t>
   </si>
   <si>
     <t>nRST</t>
@@ -106,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,18 +142,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -195,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,38 +194,28 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,18 +530,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AE9" sqref="AE9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="30" width="6.140625" customWidth="1"/>
+    <col min="1" max="30" width="6.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -664,7 +633,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -683,41 +652,41 @@
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="K2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="10" t="s">
+      <c r="L2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>15</v>
+      <c r="N2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>0</v>
+      <c r="Q2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>4</v>
@@ -740,23 +709,23 @@
       <c r="Y2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Z2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -848,7 +817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -876,318 +845,353 @@
       <c r="I4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD4" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="C11" s="10"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="C12" s="12"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-    </row>
-    <row r="17" spans="8:30" x14ac:dyDescent="0.25">
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23"/>
-    </row>
-    <row r="18" spans="8:30" x14ac:dyDescent="0.25">
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
-      <c r="AD18" s="23"/>
-    </row>
-    <row r="19" spans="8:30" x14ac:dyDescent="0.25">
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
-    </row>
-    <row r="20" spans="8:30" x14ac:dyDescent="0.25">
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="23"/>
-    </row>
-    <row r="21" spans="8:30" x14ac:dyDescent="0.25">
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
-      <c r="AC21" s="23"/>
-      <c r="AD21" s="23"/>
-    </row>
-    <row r="22" spans="8:30" x14ac:dyDescent="0.25">
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="26"/>
+      <c r="C13" s="11"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F14" s="20"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F15" s="20"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="17"/>
+    </row>
+    <row r="17" spans="6:30" x14ac:dyDescent="0.35">
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+    </row>
+    <row r="18" spans="6:30" x14ac:dyDescent="0.35">
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+    </row>
+    <row r="19" spans="6:30" x14ac:dyDescent="0.35">
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+    </row>
+    <row r="20" spans="6:30" x14ac:dyDescent="0.35">
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.0.0 schematic generated to be checked
</commit_message>
<xml_diff>
--- a/Documentation/Interface Connector Pinout.xlsx
+++ b/Documentation/Interface Connector Pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\msx\amino\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\msx\mom\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>GND</t>
   </si>
@@ -53,19 +53,19 @@
     <t>CLK</t>
   </si>
   <si>
-    <t>nRST</t>
-  </si>
-  <si>
     <t>SWD</t>
   </si>
   <si>
-    <t>SWO</t>
-  </si>
-  <si>
     <t>DIO</t>
   </si>
   <si>
     <t>USB</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>HW_VER</t>
   </si>
 </sst>
 </file>
@@ -97,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +146,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -174,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +222,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,13 +543,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="30" width="6.1796875" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="29" width="6.1796875" customWidth="1"/>
+    <col min="30" max="30" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.35">
@@ -668,10 +682,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="8" t="s">
         <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>0</v>
@@ -721,8 +735,8 @@
       <c r="AC2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="5" t="s">
-        <v>0</v>
+      <c r="AD2" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.35">
@@ -855,7 +869,7 @@
         <v>8</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>0</v>
@@ -971,7 +985,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="10"/>
       <c r="F11" s="20"/>
@@ -986,7 +1000,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="12"/>
       <c r="F12" s="20"/>
@@ -1015,6 +1029,10 @@
       <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="23"/>
       <c r="F14" s="20"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1042,6 +1060,8 @@
       <c r="AD14" s="17"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>

</xml_diff>